<commit_message>
Added favicon and ranking system
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gigabyte\Desktop\result-portal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745DAD18-3579-4700-B266-ABC924DE35C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F2AF80-6D4D-43E6-9407-36F5607013E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11532" yWindow="6204" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2157,7 +2157,7 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" ht="52.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="7">
         <v>2024331053</v>
       </c>

</xml_diff>